<commit_message>
atualização para retirar as chamadas da biblioteca locale
</commit_message>
<xml_diff>
--- a/database/ordenador_despesas.xlsx
+++ b/database/ordenador_despesas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/Programa PYQT6/pyqt6/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive\Área de Trabalho\projeto_licitacao360\licitacao360\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E9B46895-C34C-4BB1-A815-44D4D07DB29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CACA1DA0-4DE2-4901-AC93-5B1E886F83F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355074CB-FB39-48D1-B8B7-A3552C66E01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{AA7F9610-33D9-44E0-AC15-CF27201B7D9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA7F9610-33D9-44E0-AC15-CF27201B7D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <t>funcao</t>
   </si>
   <si>
-    <t>DAVID AMANCIO....</t>
+    <t>BRUNO SANTA RITA MOREIRA</t>
   </si>
 </sst>
 </file>
@@ -139,10 +139,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,17 +461,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.453125" customWidth="1"/>
-    <col min="3" max="3" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -486,9 +482,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -497,9 +493,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
atualização agentes responsáveis dispensa eletronica
</commit_message>
<xml_diff>
--- a/database/ordenador_despesas.xlsx
+++ b/database/ordenador_despesas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive\Área de Trabalho\projeto_licitacao360\licitacao360\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\Nova pasta\projeto_licitacao360\licitacao360\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355074CB-FB39-48D1-B8B7-A3552C66E01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09461067-1AD8-4943-ABD5-E8EC1387AE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA7F9610-33D9-44E0-AC15-CF27201B7D9F}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{AA7F9610-33D9-44E0-AC15-CF27201B7D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Ordenador de Despesa</t>
   </si>
@@ -60,6 +49,33 @@
   </si>
   <si>
     <t>BRUNO SANTA RITA MOREIRA</t>
+  </si>
+  <si>
+    <t>Agente Fiscal</t>
+  </si>
+  <si>
+    <t>Agente Fiscal Substituto</t>
+  </si>
+  <si>
+    <t>Capitão de Corveta (IM)</t>
+  </si>
+  <si>
+    <t>GUILHERME KIRSCHNER DE SIQUEIRA CAMPOS</t>
+  </si>
+  <si>
+    <t>Gerente de Crédito</t>
+  </si>
+  <si>
+    <t>Posto-Graduacao</t>
+  </si>
+  <si>
+    <t>NOME COMPLETO</t>
+  </si>
+  <si>
+    <t>Encarregado da Divisão de Subsistência</t>
+  </si>
+  <si>
+    <t>RAMON DE LIMA FERNANDES</t>
   </si>
 </sst>
 </file>
@@ -458,20 +474,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B528B-7B5E-4510-B870-156D10DC4C3E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -482,7 +498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -493,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -502,6 +518,50 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>